<commit_message>
feat: Implement key card eligibility and management system with dedicated service, models, and UI components.
</commit_message>
<xml_diff>
--- a/docs/Members.xlsx
+++ b/docs/Members.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnsil\Documents\GFC\cursor files\GFC-System\GFC-Studio V2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F336F5-2DC3-4B8A-80DF-9886C4973A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136DE6F2-6AC7-464F-A4B5-B55F75FE72C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F186F330-01AE-4AE8-BCC6-D9E3A3A42AC8}"/>
   </bookViews>
@@ -1626,7 +1626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1941,6 +1941,9 @@
     </xf>
     <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2260,7 +2263,7 @@
   <dimension ref="A1:S56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2279,7 +2282,7 @@
     <col min="13" max="13" width="35.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.140625" style="4" customWidth="1"/>
     <col min="15" max="15" width="21.28515625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="110.7109375" customWidth="1"/>
   </cols>
@@ -2350,7 +2353,7 @@
       </c>
       <c r="E2"/>
       <c r="F2" s="110" t="s">
-        <v>399</v>
+        <v>142</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>400</v>
@@ -2379,8 +2382,8 @@
       <c r="O2" s="9">
         <v>39653</v>
       </c>
-      <c r="P2" s="9">
-        <v>39653</v>
+      <c r="P2" s="111">
+        <v>25707</v>
       </c>
       <c r="Q2" s="35" t="s">
         <v>143</v>
@@ -2397,7 +2400,7 @@
       </c>
       <c r="E3"/>
       <c r="F3" s="6" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>411</v>
@@ -2422,8 +2425,8 @@
       <c r="O3" s="9">
         <v>37161</v>
       </c>
-      <c r="P3" s="9">
-        <v>37161</v>
+      <c r="P3" s="111">
+        <v>25225</v>
       </c>
       <c r="Q3" s="35" t="s">
         <v>144</v>
@@ -2442,7 +2445,7 @@
       </c>
       <c r="E4"/>
       <c r="F4" s="6" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>415</v>
@@ -2469,8 +2472,8 @@
       <c r="O4" s="9">
         <v>35773</v>
       </c>
-      <c r="P4" s="9">
-        <v>35773</v>
+      <c r="P4" s="111">
+        <v>24886</v>
       </c>
       <c r="Q4" s="35" t="s">
         <v>144</v>
@@ -2487,7 +2490,7 @@
       </c>
       <c r="E5"/>
       <c r="F5" s="6" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>420</v>
@@ -2516,8 +2519,8 @@
       <c r="O5" s="9">
         <v>40015</v>
       </c>
-      <c r="P5" s="9">
-        <v>40015</v>
+      <c r="P5" s="111">
+        <v>27744</v>
       </c>
       <c r="Q5" s="35" t="s">
         <v>144</v>
@@ -2536,7 +2539,7 @@
       </c>
       <c r="E6"/>
       <c r="F6" s="6" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>425</v>
@@ -2565,8 +2568,8 @@
       <c r="O6" s="102">
         <v>41571</v>
       </c>
-      <c r="P6" s="102">
-        <v>41571</v>
+      <c r="P6" s="111">
+        <v>24414</v>
       </c>
       <c r="Q6" s="35" t="s">
         <v>144</v>
@@ -2585,7 +2588,7 @@
       </c>
       <c r="E7"/>
       <c r="F7" s="6" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>430</v>
@@ -2612,8 +2615,8 @@
       <c r="O7" s="9">
         <v>42781</v>
       </c>
-      <c r="P7" s="9">
-        <v>42781</v>
+      <c r="P7" s="111">
+        <v>24969</v>
       </c>
       <c r="Q7" s="35" t="s">
         <v>144</v>
@@ -2632,7 +2635,7 @@
       </c>
       <c r="E8"/>
       <c r="F8" s="6" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>435</v>
@@ -2659,8 +2662,8 @@
       <c r="O8" s="9">
         <v>39226</v>
       </c>
-      <c r="P8" s="9">
-        <v>39226</v>
+      <c r="P8" s="111">
+        <v>26516</v>
       </c>
       <c r="Q8" s="35" t="s">
         <v>144</v>
@@ -7209,10 +7212,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26AA510-3AF6-4344-9BE8-EF0864DE267D}">
-  <dimension ref="A1:Y24"/>
+  <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:Q9"/>
+      <selection activeCell="P3" sqref="P3:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7222,14 +7225,15 @@
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="24" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="12.42578125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="30.85546875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="30.85546875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="0" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
@@ -7334,8 +7338,8 @@
       <c r="O3" s="9">
         <v>39653</v>
       </c>
-      <c r="P3" s="9">
-        <v>39653</v>
+      <c r="P3" s="111">
+        <v>25707</v>
       </c>
       <c r="Q3" s="35" t="s">
         <v>143</v>
@@ -7374,8 +7378,8 @@
       <c r="O4" s="9">
         <v>37161</v>
       </c>
-      <c r="P4" s="9">
-        <v>37161</v>
+      <c r="P4" s="111">
+        <v>25225</v>
       </c>
       <c r="Q4" s="35" t="s">
         <v>144</v>
@@ -7419,8 +7423,8 @@
       <c r="O5" s="9">
         <v>35773</v>
       </c>
-      <c r="P5" s="9">
-        <v>35773</v>
+      <c r="P5" s="111">
+        <v>24886</v>
       </c>
       <c r="Q5" s="35" t="s">
         <v>144</v>
@@ -7463,8 +7467,8 @@
       <c r="O6" s="9">
         <v>40015</v>
       </c>
-      <c r="P6" s="9">
-        <v>40015</v>
+      <c r="P6" s="111">
+        <v>27744</v>
       </c>
       <c r="Q6" s="35" t="s">
         <v>144</v>
@@ -7510,8 +7514,8 @@
       <c r="O7" s="102">
         <v>41571</v>
       </c>
-      <c r="P7" s="102">
-        <v>41571</v>
+      <c r="P7" s="111">
+        <v>24414</v>
       </c>
       <c r="Q7" s="35" t="s">
         <v>144</v>
@@ -7555,8 +7559,8 @@
       <c r="O8" s="9">
         <v>42781</v>
       </c>
-      <c r="P8" s="9">
-        <v>42781</v>
+      <c r="P8" s="111">
+        <v>24969</v>
       </c>
       <c r="Q8" s="35" t="s">
         <v>144</v>
@@ -7600,8 +7604,8 @@
       <c r="O9" s="9">
         <v>39226</v>
       </c>
-      <c r="P9" s="9">
-        <v>39226</v>
+      <c r="P9" s="111">
+        <v>26516</v>
       </c>
       <c r="Q9" s="35" t="s">
         <v>144</v>
@@ -7609,6 +7613,32 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="Q10" s="35"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
@@ -7618,7 +7648,6 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -7637,82 +7666,55 @@
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-    </row>
-    <row r="20" spans="1:25" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="106" t="s">
+    <row r="19" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="106" t="s">
         <v>398</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C19" t="s">
         <v>439</v>
       </c>
-      <c r="D20" s="106" t="s">
+      <c r="D19" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="F20" s="108" t="s">
+      <c r="F19" s="108" t="s">
         <v>172</v>
       </c>
-      <c r="G20" s="106" t="s">
+      <c r="G19" s="106" t="s">
         <v>404</v>
       </c>
-      <c r="H20" s="106" t="s">
+      <c r="H19" s="106" t="s">
         <v>405</v>
       </c>
-      <c r="I20" s="106" t="s">
+      <c r="I19" s="106" t="s">
         <v>406</v>
       </c>
-      <c r="J20" s="107">
+      <c r="J19" s="107">
         <v>39560</v>
       </c>
-      <c r="K20" s="107" t="s">
+      <c r="K19" s="107" t="s">
         <v>33</v>
       </c>
-      <c r="L20" s="107" t="s">
+      <c r="L19" s="107" t="s">
         <v>407</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M19" t="s">
         <v>408</v>
       </c>
-      <c r="N20" s="109">
+      <c r="N19" s="109">
         <v>38746</v>
       </c>
-      <c r="O20" s="109">
+      <c r="O19" s="109">
         <v>38771</v>
       </c>
-      <c r="P20" s="109">
+      <c r="P19" s="109">
         <v>38771</v>
       </c>
-      <c r="Q20" s="35" t="s">
+      <c r="Q19" s="35" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="E24" t="s">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
         <v>438</v>
       </c>
     </row>

</xml_diff>